<commit_message>
Refactor configuration loading and enhance postage validation in Excel parsing
</commit_message>
<xml_diff>
--- a/packages/event-builder/examples/specifications.xlsx
+++ b/packages/event-builder/examples/specifications.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.houston/nhs-notify/nhs-notify-supplier-config/packages/events/src/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.houston/nhs-notify/nhs-notify-supplier-config/packages/event-builder/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89186C5-4D98-924C-8414-6B472FBC3AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431C7B3A-5EEB-814A-B940-188A25EFFBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7580" yWindow="-26580" windowWidth="34560" windowHeight="21660" activeTab="1" xr2:uid="{7C1C9A7A-5291-284B-B7CE-72455DFF925E}"/>
+    <workbookView xWindow="-25520" yWindow="-31780" windowWidth="60060" windowHeight="31780" activeTab="1" xr2:uid="{7C1C9A7A-5291-284B-B7CE-72455DFF925E}"/>
   </bookViews>
   <sheets>
     <sheet name="LetterVariant" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -174,22 +174,22 @@
     <t>postage.maxSheets</t>
   </si>
   <si>
-    <t>economy</t>
-  </si>
-  <si>
-    <t>articles-blind</t>
-  </si>
-  <si>
-    <t>firstclass</t>
-  </si>
-  <si>
-    <t>admail</t>
-  </si>
-  <si>
     <t>postage.size</t>
   </si>
   <si>
     <t>LARGE</t>
+  </si>
+  <si>
+    <t>ECONOMY</t>
+  </si>
+  <si>
+    <t>FIRST</t>
+  </si>
+  <si>
+    <t>ARTICLES_BLIND</t>
+  </si>
+  <si>
+    <t>postage.deliverySLA</t>
   </si>
 </sst>
 </file>
@@ -718,27 +718,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F391B7A5-CD97-A14C-80A9-E44FAC84811F}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -773,10 +775,13 @@
         <v>44</v>
       </c>
       <c r="L1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -799,7 +804,7 @@
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K2">
         <v>5</v>
@@ -807,8 +812,11 @@
       <c r="L2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -831,16 +839,19 @@
         <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K3">
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -863,7 +874,7 @@
         <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="K4">
         <v>5</v>
@@ -871,8 +882,11 @@
       <c r="L4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -895,7 +909,7 @@
         <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="K5">
         <v>5</v>
@@ -903,8 +917,11 @@
       <c r="L5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -927,7 +944,7 @@
         <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K6">
         <v>5</v>
@@ -935,8 +952,11 @@
       <c r="L6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -965,13 +985,16 @@
         <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="K7">
         <v>4</v>
       </c>
       <c r="L7" t="s">
         <v>37</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature: Introduce volume group event builder and update related tests
</commit_message>
<xml_diff>
--- a/packages/event-builder/examples/specifications.xlsx
+++ b/packages/event-builder/examples/specifications.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.houston/nhs-notify/nhs-notify-supplier-config/packages/event-builder/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0040C1-6C3F-2B47-9A49-8DE274C6A9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178A195A-FA87-1446-A63E-43E6179CFC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3840" yWindow="-31780" windowWidth="38400" windowHeight="31780" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3840" yWindow="-31780" windowWidth="38400" windowHeight="31780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PackSpecification" sheetId="1" r:id="rId1"/>
     <sheet name="LetterVariant" sheetId="2" r:id="rId2"/>
-    <sheet name="Contract" sheetId="3" r:id="rId3"/>
+    <sheet name="VolumeGroup" sheetId="3" r:id="rId3"/>
     <sheet name="Supplier" sheetId="4" r:id="rId4"/>
     <sheet name="SupplierAllocation" sheetId="5" r:id="rId5"/>
     <sheet name="SupplierPack" sheetId="6" r:id="rId6"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="129">
   <si>
     <t>id</t>
   </si>
@@ -111,9 +111,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>contractId</t>
-  </si>
-  <si>
     <t>packSpecificationIds</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>channelType</t>
   </si>
   <si>
-    <t>contract</t>
-  </si>
-  <si>
     <t>supplier</t>
   </si>
   <si>
@@ -412,6 +406,12 @@
   </si>
   <si>
     <t>DISABLED</t>
+  </si>
+  <si>
+    <t>volumeGroupId</t>
+  </si>
+  <si>
+    <t>dailyCapacity</t>
   </si>
 </sst>
 </file>
@@ -918,40 +918,40 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
         <v>69</v>
       </c>
-      <c r="E2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
-      </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J2">
         <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M2">
         <v>20</v>
@@ -966,66 +966,66 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" t="s">
         <v>86</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>87</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>88</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>89</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>90</v>
       </c>
-      <c r="V2" t="s">
-        <v>91</v>
-      </c>
-      <c r="W2" t="s">
-        <v>92</v>
-      </c>
       <c r="X2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Z2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J3">
         <v>3</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M3">
         <v>5</v>
@@ -1040,54 +1040,54 @@
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="R3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="U3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="V3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="W3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="X3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Z3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1105,54 +1105,54 @@
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S4" t="s">
+        <v>92</v>
+      </c>
+      <c r="T4" t="s">
+        <v>93</v>
+      </c>
+      <c r="U4" t="s">
         <v>94</v>
       </c>
-      <c r="T4" t="s">
-        <v>95</v>
-      </c>
-      <c r="U4" t="s">
-        <v>96</v>
-      </c>
       <c r="V4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="W4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="X4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Z4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J5">
         <v>3</v>
@@ -1170,45 +1170,45 @@
         <v>0</v>
       </c>
       <c r="S5" t="s">
+        <v>86</v>
+      </c>
+      <c r="U5" t="s">
         <v>88</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
+        <v>89</v>
+      </c>
+      <c r="W5" t="s">
         <v>90</v>
       </c>
-      <c r="V5" t="s">
-        <v>91</v>
-      </c>
-      <c r="W5" t="s">
-        <v>92</v>
-      </c>
       <c r="X5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1226,51 +1226,51 @@
         <v>0</v>
       </c>
       <c r="Q6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="S6" t="s">
+        <v>86</v>
+      </c>
+      <c r="U6" t="s">
         <v>88</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
+        <v>89</v>
+      </c>
+      <c r="W6" t="s">
         <v>90</v>
       </c>
-      <c r="V6" t="s">
-        <v>91</v>
-      </c>
-      <c r="W6" t="s">
-        <v>92</v>
-      </c>
       <c r="X6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Z6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J7">
         <v>3</v>
@@ -1288,34 +1288,34 @@
         <v>20</v>
       </c>
       <c r="Q7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R7" t="s">
+        <v>96</v>
+      </c>
+      <c r="S7" t="s">
+        <v>97</v>
+      </c>
+      <c r="T7" t="s">
         <v>98</v>
       </c>
-      <c r="S7" t="s">
-        <v>99</v>
-      </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
+        <v>80</v>
+      </c>
+      <c r="V7" t="s">
+        <v>89</v>
+      </c>
+      <c r="W7" t="s">
+        <v>90</v>
+      </c>
+      <c r="X7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="U7" t="s">
-        <v>82</v>
-      </c>
-      <c r="V7" t="s">
-        <v>91</v>
-      </c>
-      <c r="W7" t="s">
-        <v>92</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="Y7" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z7" t="s">
         <v>103</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1330,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1339,7 +1339,7 @@
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -1361,22 +1361,22 @@
         <v>27</v>
       </c>
       <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
       <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
         <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
       </c>
       <c r="J1" t="s">
         <v>12</v>
@@ -1393,25 +1393,25 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
       </c>
       <c r="J2">
         <v>20</v>
@@ -1425,25 +1425,25 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>49</v>
       </c>
-      <c r="D3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" t="s">
-        <v>51</v>
-      </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J3">
         <v>5</v>
@@ -1457,25 +1457,25 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J4">
         <v>5</v>
@@ -1489,25 +1489,25 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" t="s">
-        <v>59</v>
-      </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J5">
         <v>5</v>
@@ -1521,31 +1521,31 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
         <v>60</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" t="s">
+      <c r="I6" t="s">
         <v>62</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" t="s">
-        <v>64</v>
       </c>
       <c r="J6">
         <v>4</v>
@@ -1560,7 +1560,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:M1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C1 E1:M1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1589,10 +1589,10 @@
         <v>27</v>
       </c>
       <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
         <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1600,24 +1600,24 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1630,15 +1630,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1646,29 +1653,47 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="D2">
+        <v>500000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="D3">
+        <v>500000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1684,13 +1709,13 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
@@ -1701,13 +1726,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1715,59 +1740,59 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2">
         <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D3">
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D4">
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 C1:E1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1776,7 +1801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1793,10 +1818,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1804,156 +1829,156 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>